<commit_message>
Update returns data with 개방형 랩 rename applied
Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -70141,6 +70141,9 @@
           <t>24.6%</t>
         </is>
       </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr">
         <is>
           <t>24.6%</t>
@@ -70161,11 +70164,21 @@
           <t>21.6%</t>
         </is>
       </c>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr">
         <is>
           <t>21.6%</t>
         </is>
       </c>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -70293,6 +70306,9 @@
           <t>15.6%</t>
         </is>
       </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr">
         <is>
           <t>23.0%</t>
@@ -70313,11 +70329,20 @@
           <t>17.6%</t>
         </is>
       </c>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="inlineStr">
         <is>
           <t>17.9%</t>
         </is>
       </c>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
       <c r="AQ3" t="inlineStr">
         <is>
           <t>0.0%</t>

</xml_diff>

<commit_message>
Fix report date to use most common latest date across columns
Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -69790,7 +69790,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ3"/>
+  <dimension ref="A1:AQ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -70349,6 +70349,175 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-0.6%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-0.2%</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>19.8%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>42.0%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>54.7%</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>108.5%</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>26.4%</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-0.6%</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>-0.2%</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>19.8%</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>38.0%</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>50.3%</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>102.6%</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>26.4%</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>-0.6%</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>1.2%</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>20.3%</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>33.5%</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>45.7%</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>106.7%</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>26.9%</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>0.1%</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>0.3%</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>15.6%</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>23.0%</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>-1.1%</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>-2.5%</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>17.6%</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>17.9%</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update: Wrap_NAV.xlsx (2026-02-19 14:16)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Antigravity_Market_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27499244-549D-4589-924E-1191DFB5DE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DF9EDC-F6BC-44D3-8FDE-2E4E6AA1ABBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19904,7 +19904,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H469"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
+      <selection activeCell="H360" sqref="H360"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
update: Wrap_NAV.xlsx (2026-02-19 14:33)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Antigravity_Market_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C48325-D8C1-495D-90DB-1B26BD0A0E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD73E2A-ECBF-4762-9880-9962178E5007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW" sheetId="1" r:id="rId1"/>
@@ -19904,8 +19904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G483"/>
   <sheetViews>
-    <sheetView topLeftCell="A446" workbookViewId="0">
-      <selection activeCell="D469" sqref="D469"/>
+    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
+      <selection activeCell="E483" sqref="E483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -42781,7 +42781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2796"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2749" workbookViewId="0">
+    <sheetView topLeftCell="A2749" workbookViewId="0">
       <selection activeCell="D2796" sqref="D2796"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update: Wrap_NAV.xlsx (2026-02-19 16:13)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Antigravity_Market_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC11500-F4F2-4E39-89FB-BA831B51D739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98BCFC5-690A-455A-AC9C-717E90BB2E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW" sheetId="1" r:id="rId1"/>
@@ -19967,8 +19967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
-      <selection activeCell="E483" sqref="E483"/>
+    <sheetView topLeftCell="A443" workbookViewId="0">
+      <selection activeCell="A483" sqref="A483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -31102,8 +31102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G716"/>
   <sheetViews>
-    <sheetView topLeftCell="A669" workbookViewId="0">
-      <selection activeCell="A716" sqref="A716"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update: Wrap_NAV.xlsx (2026-02-19 16:17)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Antigravity_Market_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DA9AC0-D135-422E-965C-953A76D58686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D926DB-21A5-47A4-A438-BD04D80470C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31118,7 +31118,7 @@
   <dimension ref="A1:AA716"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update: Wrap_NAV.xlsx (2026-02-20 16:20)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Antigravity_Market_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76EE333-CDE1-4BEA-BAFD-6073F3756115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C6072D-6410-4D56-8B4E-C1646736D7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31195,8 +31195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A668" workbookViewId="0">
-      <selection activeCell="E715" sqref="E715"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update: Wrap_NAV.xlsx (2026-02-23 10:45)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Antigravity_Market_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A54B6EF-17F1-4C6C-A5FF-3A242D29DCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17FDFFE-3E88-4CE0-BD2D-71748088130D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,20 @@
     <sheet name="Code" sheetId="3" r:id="rId3"/>
     <sheet name="수익률" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -19634,7 +19647,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -19677,6 +19690,30 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -19752,10 +19789,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -19791,8 +19831,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="백분율" xfId="1" builtinId="5"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -31596,10 +31640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G715"/>
+  <dimension ref="A1:G716"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A668" workbookViewId="0">
-      <selection activeCell="D715" sqref="D715"/>
+    <sheetView tabSelected="1" topLeftCell="A670" workbookViewId="0">
+      <selection activeCell="A714" sqref="A714"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -44373,7 +44417,7 @@
       <c r="B682">
         <v>2021.31</v>
       </c>
-      <c r="C682">
+      <c r="C682" s="13">
         <v>2038.06</v>
       </c>
       <c r="D682">
@@ -44393,7 +44437,7 @@
       <c r="B683">
         <v>2089.4899999999998</v>
       </c>
-      <c r="C683">
+      <c r="C683" s="14">
         <v>2047.3</v>
       </c>
       <c r="D683">
@@ -45060,6 +45104,11 @@
       <c r="G715">
         <v>1024.43</v>
       </c>
+    </row>
+    <row r="716" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B716" s="15"/>
+      <c r="C716" s="15"/>
+      <c r="D716" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
update: Wrap_NAV.xlsx (2026-02-23 10:46)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Antigravity_Market_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17FDFFE-3E88-4CE0-BD2D-71748088130D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E020C9D-444C-4B1C-9CFE-7D7C3BBA1D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31643,7 +31643,7 @@
   <dimension ref="A1:G716"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A670" workbookViewId="0">
-      <selection activeCell="A714" sqref="A714"/>
+      <selection activeCell="F695" sqref="F695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update: Wrap_NAV.xlsx (2026-02-23 11:02)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Antigravity_Market_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E020C9D-444C-4B1C-9CFE-7D7C3BBA1D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B197898A-50DD-4467-BB6B-DC25B788CB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31642,8 +31642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G716"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A670" workbookViewId="0">
-      <selection activeCell="F695" sqref="F695"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update Wrap_NAV (2026-02-25 06:40)
</commit_message>
<xml_diff>
--- a/Wrap_NAV.xlsx
+++ b/Wrap_NAV.xlsx
@@ -17048,7 +17048,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G717"/>
+  <dimension ref="A1:G718"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32003,6 +32003,31 @@
       </c>
       <c r="G717" t="n">
         <v>1060.47</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="16" t="inlineStr">
+        <is>
+          <t>2026-02-25</t>
+        </is>
+      </c>
+      <c r="B718" t="n">
+        <v>3036.05</v>
+      </c>
+      <c r="C718" t="n">
+        <v>2974.72</v>
+      </c>
+      <c r="D718" t="n">
+        <v>2290.36</v>
+      </c>
+      <c r="E718" t="n">
+        <v>6093.33</v>
+      </c>
+      <c r="F718" t="n">
+        <v>1165.73</v>
+      </c>
+      <c r="G718" t="n">
+        <v>1079.98</v>
       </c>
     </row>
   </sheetData>
@@ -98022,7 +98047,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ10"/>
+  <dimension ref="A1:AQ11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -99900,6 +99925,207 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-02-25</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1.9%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>9.8%</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>27.1%</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>73.8%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>82.3%</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>134.9%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>50.2%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1.9%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>9.8%</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>27.1%</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>68.9%</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>128.2%</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>46.0%</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>1.9%</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>9.8%</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>27.3%</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>62.5%</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>71.9%</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>131.6%</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>50.8%</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>2.1%</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>10.6%</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>22.1%</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>57.9%</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>89.8%</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>131.7%</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>44.6%</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>0.1%</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>5.4%</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>17.3%</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>36.2%</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>46.1%</t>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>51.5%</t>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>26.0%</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>1.8%</t>
+        </is>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t>8.2%</t>
+        </is>
+      </c>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr">
+        <is>
+          <t>8.0%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>